<commit_message>
Excel summary of results
</commit_message>
<xml_diff>
--- a/Data/Generated New/Graph List and Stats.xlsx
+++ b/Data/Generated New/Graph List and Stats.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Generated New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D15E815-3EF2-422D-AB25-2DFC97ACA9E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644B907C-C36C-45C9-9E7B-017B8CACCEA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="180" windowWidth="16464" windowHeight="13608" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
+    <workbookView xWindow="24324" yWindow="228" windowWidth="21252" windowHeight="13608" activeTab="2" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AdjList" sheetId="1" r:id="rId1"/>
+    <sheet name="AdjMat" sheetId="2" r:id="rId2"/>
+    <sheet name="IncMat" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="65">
   <si>
     <t>Filename</t>
   </si>
@@ -220,6 +222,15 @@
   </si>
   <si>
     <t>khop average time (50 iterations)</t>
+  </si>
+  <si>
+    <t>100 Additions</t>
+  </si>
+  <si>
+    <t>100 Deletions</t>
+  </si>
+  <si>
+    <t>khop average time (average taken from 50 iterations)</t>
   </si>
 </sst>
 </file>
@@ -263,9 +274,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D71CDE3-7DBD-462C-93FC-85AE65D9340E}">
-  <dimension ref="B1:I57"/>
+  <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,14 +604,17 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,8 +636,14 @@
       <c r="I2" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -632,8 +653,17 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>1.9065019999999999E-5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.2874765999999901E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4.6680257999999898E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -643,8 +673,17 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>3.5581119999999999E-5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5.4121759999999998E-5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.3750067999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -654,8 +693,17 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>3.5935739999999998E-5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.0210876E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6.7331398000000002E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -665,8 +713,17 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>1.3815955999999999E-4</v>
+      </c>
+      <c r="G6">
+        <v>1.5738910399999901E-3</v>
+      </c>
+      <c r="H6">
+        <v>3.912428448E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -676,8 +733,17 @@
       <c r="D7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>1.5165907999999901E-4</v>
+      </c>
+      <c r="G7">
+        <v>1.2920079399999999E-3</v>
+      </c>
+      <c r="H7">
+        <v>4.0837181179999897E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -687,8 +753,17 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>1.47865259999999E-4</v>
+      </c>
+      <c r="G8">
+        <v>1.4386027999999901E-3</v>
+      </c>
+      <c r="H8">
+        <v>4.536798014E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -698,8 +773,17 @@
       <c r="D9">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>3.5549925999999902E-4</v>
+      </c>
+      <c r="G9">
+        <v>7.3032138799999898E-3</v>
+      </c>
+      <c r="H9">
+        <v>0.29823591620000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -709,8 +793,17 @@
       <c r="D10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>3.0862549999999901E-4</v>
+      </c>
+      <c r="G10">
+        <v>8.1232519199999909E-3</v>
+      </c>
+      <c r="H10">
+        <v>0.34319052485999901</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -720,8 +813,17 @@
       <c r="D11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>2.5940251999999998E-4</v>
+      </c>
+      <c r="G11">
+        <v>6.5360263E-3</v>
+      </c>
+      <c r="H11">
+        <v>0.29742041835999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -731,8 +833,17 @@
       <c r="D12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>8.3084299999999905E-5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.1271156E-4</v>
+      </c>
+      <c r="H12">
+        <v>5.2149841379999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -742,8 +853,17 @@
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>2.03581599999999E-5</v>
+      </c>
+      <c r="G13">
+        <v>3.38502115999999E-3</v>
+      </c>
+      <c r="H13">
+        <v>2.3810141140000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -753,8 +873,17 @@
       <c r="D14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>4.8817080000000003E-5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>6.9245915999999901E-4</v>
+      </c>
+      <c r="H14">
+        <v>2.2179341419999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -764,8 +893,17 @@
       <c r="D15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>9.5409119999999899E-4</v>
+      </c>
+      <c r="G15">
+        <v>4.0299784140000003E-2</v>
+      </c>
+      <c r="H15">
+        <v>2.3086100533199998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -775,8 +913,17 @@
       <c r="D16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>3.79050879999999E-4</v>
+      </c>
+      <c r="G16">
+        <v>9.4397791119999894E-2</v>
+      </c>
+      <c r="H16">
+        <v>3.0831228558400001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -786,8 +933,17 @@
       <c r="D17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>1.22966896E-3</v>
+      </c>
+      <c r="G17">
+        <v>9.2360808459999902E-2</v>
+      </c>
+      <c r="H17">
+        <v>6.2140992448799999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -797,8 +953,17 @@
       <c r="D18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>4.6542970399999902E-3</v>
+      </c>
+      <c r="G18">
+        <v>0.71137995225999995</v>
+      </c>
+      <c r="H18">
+        <v>32.387339088860003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -808,8 +973,17 @@
       <c r="D19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>3.7389373E-3</v>
+      </c>
+      <c r="G19">
+        <v>0.66090156169999903</v>
+      </c>
+      <c r="H19">
+        <v>28.8205005797799</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -819,8 +993,17 @@
       <c r="D20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>4.9022734599999899E-3</v>
+      </c>
+      <c r="G20">
+        <v>0.29517676047999902</v>
+      </c>
+      <c r="H20">
+        <v>17.050284592560001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -830,8 +1013,17 @@
       <c r="D21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F21" s="2">
+        <v>1.2433879999999899E-4</v>
+      </c>
+      <c r="G21">
+        <v>3.1110507199999999E-3</v>
+      </c>
+      <c r="H21">
+        <v>5.8952841199999897E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -841,8 +1033,17 @@
       <c r="D22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F22" s="2">
+        <v>1.19383679999999E-4</v>
+      </c>
+      <c r="G22">
+        <v>1.7303143400000001E-3</v>
+      </c>
+      <c r="H22">
+        <v>5.7988563819999901E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -852,8 +1053,17 @@
       <c r="D23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F23" s="2">
+        <v>5.78839799999999E-5</v>
+      </c>
+      <c r="G23">
+        <v>3.1328508999999998E-3</v>
+      </c>
+      <c r="H23">
+        <v>3.4127632319999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -863,8 +1073,17 @@
       <c r="D24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F24" s="2">
+        <v>8.8710432000000002E-4</v>
+      </c>
+      <c r="G24">
+        <v>0.20491251206</v>
+      </c>
+      <c r="H24">
+        <v>11.3893343637</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -874,8 +1093,17 @@
       <c r="D25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F25" s="2">
+        <v>4.2155972E-4</v>
+      </c>
+      <c r="G25">
+        <v>0.18960721517999901</v>
+      </c>
+      <c r="H25">
+        <v>8.6356112273600001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -886,7 +1114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -897,7 +1125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -908,7 +1136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -919,7 +1147,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -929,8 +1157,17 @@
       <c r="D31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F31" s="2">
+        <v>1.5405439999999999E-5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2.0673979999999899E-5</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3.7747419999999998E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -940,8 +1177,17 @@
       <c r="D32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F32" s="2">
+        <v>1.7479259999999899E-5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.892482E-5</v>
+      </c>
+      <c r="H32" s="2">
+        <v>4.1874739999999997E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -951,8 +1197,17 @@
       <c r="D33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F33" s="2">
+        <v>2.6030919999999902E-5</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.9846039999999999E-5</v>
+      </c>
+      <c r="H33" s="2">
+        <v>4.8186219999999998E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -962,8 +1217,17 @@
       <c r="D34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F34" s="2">
+        <v>8.4476480000000002E-5</v>
+      </c>
+      <c r="G34" s="2">
+        <v>4.4106119999999998E-4</v>
+      </c>
+      <c r="H34">
+        <v>4.8287935200000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -973,8 +1237,17 @@
       <c r="D35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F35" s="2">
+        <v>8.7517979999999997E-5</v>
+      </c>
+      <c r="G35" s="2">
+        <v>4.7416071999999902E-4</v>
+      </c>
+      <c r="H35">
+        <v>4.9460617199999996E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -984,8 +1257,17 @@
       <c r="D36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F36" s="2">
+        <v>1.0575639999999901E-4</v>
+      </c>
+      <c r="G36" s="2">
+        <v>5.7108691999999996E-4</v>
+      </c>
+      <c r="H36">
+        <v>5.3350818400000003E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -995,8 +1277,17 @@
       <c r="D37">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F37" s="2">
+        <v>3.1755979999999997E-4</v>
+      </c>
+      <c r="G37">
+        <v>4.6868342E-3</v>
+      </c>
+      <c r="H37">
+        <v>7.8076669840000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1006,8 +1297,17 @@
       <c r="D38">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F38" s="2">
+        <v>2.40064339999999E-4</v>
+      </c>
+      <c r="G38">
+        <v>4.4979749599999997E-3</v>
+      </c>
+      <c r="H38">
+        <v>7.806480214E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -1017,8 +1317,17 @@
       <c r="D39">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F39" s="2">
+        <v>2.6090108000000002E-4</v>
+      </c>
+      <c r="G39">
+        <v>4.2891689999999903E-3</v>
+      </c>
+      <c r="H39">
+        <v>8.1796734119999895E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -1028,8 +1337,17 @@
       <c r="D40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F40" s="2">
+        <v>2.0091639999999999E-5</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2.5213119999999901E-5</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2.8549580000000001E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -1039,8 +1357,17 @@
       <c r="D41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F41" s="2">
+        <v>1.86311399999999E-5</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.8227219999999999E-5</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2.7684240000000001E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -1050,8 +1377,17 @@
       <c r="D42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F42" s="2">
+        <v>1.8075559999999899E-5</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1.95672999999999E-5</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2.0396439999999901E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -1061,8 +1397,17 @@
       <c r="D43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F43" s="2">
+        <v>1.0065494E-4</v>
+      </c>
+      <c r="G43" s="2">
+        <v>9.4824611999999998E-4</v>
+      </c>
+      <c r="H43">
+        <v>4.8438676959999899E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -1072,8 +1417,17 @@
       <c r="D44">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F44" s="2">
+        <v>1.0043999999999999E-4</v>
+      </c>
+      <c r="G44">
+        <v>1.6053611999999899E-3</v>
+      </c>
+      <c r="H44">
+        <v>3.8956613700000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -1083,8 +1437,17 @@
       <c r="D45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F45" s="2">
+        <v>9.1473559999999995E-5</v>
+      </c>
+      <c r="G45" s="2">
+        <v>8.4395703999999897E-4</v>
+      </c>
+      <c r="H45">
+        <v>4.1313744479999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -1094,8 +1457,17 @@
       <c r="D46">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F46" s="2">
+        <v>3.4440707999999998E-4</v>
+      </c>
+      <c r="G46">
+        <v>3.7451472620000002E-2</v>
+      </c>
+      <c r="H46">
+        <v>1.3609141785799901</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -1105,8 +1477,17 @@
       <c r="D47">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F47" s="2">
+        <v>3.3002681999999897E-4</v>
+      </c>
+      <c r="G47">
+        <v>4.1407055720000002E-2</v>
+      </c>
+      <c r="H47">
+        <v>1.23728365578</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -1116,8 +1497,17 @@
       <c r="D48">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F48" s="2">
+        <v>3.4391093999999999E-4</v>
+      </c>
+      <c r="G48">
+        <v>3.9971098699999999E-2</v>
+      </c>
+      <c r="H48">
+        <v>1.21835427683999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -1127,8 +1517,17 @@
       <c r="D49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F49" s="2">
+        <v>2.1724459999999901E-5</v>
+      </c>
+      <c r="G49" s="2">
+        <v>2.313576E-5</v>
+      </c>
+      <c r="H49" s="2">
+        <v>3.8763999999999997E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -1138,8 +1537,17 @@
       <c r="D50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F50" s="2">
+        <v>2.3319379999999899E-5</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2.893554E-5</v>
+      </c>
+      <c r="H50" s="2">
+        <v>4.8773879999999901E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -1149,8 +1557,17 @@
       <c r="D51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F51" s="2">
+        <v>2.0726699999999901E-5</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2.9280359999999999E-5</v>
+      </c>
+      <c r="H51" s="2">
+        <v>5.0324279999999899E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -1160,8 +1577,17 @@
       <c r="D52">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F52" s="2">
+        <v>1.1482538E-4</v>
+      </c>
+      <c r="G52">
+        <v>1.0397177599999999E-3</v>
+      </c>
+      <c r="H52">
+        <v>6.9941663900000006E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -1171,8 +1597,17 @@
       <c r="D53">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F53" s="2">
+        <v>9.2418839999999905E-5</v>
+      </c>
+      <c r="G53">
+        <v>1.26489913999999E-3</v>
+      </c>
+      <c r="H53">
+        <v>6.6037970539999893E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -1183,7 +1618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -1194,7 +1629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -1205,7 +1640,2141 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>10000</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE147AB4-93A1-4224-A52F-043C7AD8859B}">
+  <dimension ref="B1:L57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.1749195999999999E-4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9.5037665999999905E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5.0696548000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.3971880000000002E-4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>7.8653029999999904E-4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.32227457999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.1021735999999899E-4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5.0234737999999999E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6.2013390599999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.5016021999999905E-4</v>
+      </c>
+      <c r="G6">
+        <v>4.0946343999999999E-3</v>
+      </c>
+      <c r="H6">
+        <v>4.0904141739999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.7788712000000002E-4</v>
+      </c>
+      <c r="G7">
+        <v>8.1478149599999907E-3</v>
+      </c>
+      <c r="H7">
+        <v>9.61732805E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6.6913071999999895E-4</v>
+      </c>
+      <c r="G8">
+        <v>5.2488585599999998E-3</v>
+      </c>
+      <c r="H8">
+        <v>6.6781945299999895E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8.1939527999999996E-4</v>
+      </c>
+      <c r="G9">
+        <v>1.282707286E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.49750794745999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8.9658399999999997E-4</v>
+      </c>
+      <c r="G10">
+        <v>1.6878596159999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.26222596496</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>500</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.0397159200000001E-3</v>
+      </c>
+      <c r="G11">
+        <v>1.7394373299999901E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.46647592725999998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>5000</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.4966243600000001E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.7595001999999999E-3</v>
+      </c>
+      <c r="H12">
+        <v>7.3398038919999894E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>5000</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.7983590399999901E-3</v>
+      </c>
+      <c r="G13">
+        <v>2.4855909800000002E-3</v>
+      </c>
+      <c r="H13">
+        <v>0.117171630979999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5000</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.36588967999999E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5.9872543199999996E-3</v>
+      </c>
+      <c r="H14">
+        <v>4.5263969739999903E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>5000</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2.5829122799999999E-3</v>
+      </c>
+      <c r="G15">
+        <v>9.2259297279999999E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.7530737077999996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>5000</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.38975596E-3</v>
+      </c>
+      <c r="G16">
+        <v>5.7213859040000002E-2</v>
+      </c>
+      <c r="H16">
+        <v>5.8970220660199901</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>5000</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>2.3034924199999999E-3</v>
+      </c>
+      <c r="G17">
+        <v>4.7836249980000002E-2</v>
+      </c>
+      <c r="H17">
+        <v>6.4239563367199999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>5000</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>5.5844965199999897E-3</v>
+      </c>
+      <c r="G18">
+        <v>0.46205770268000002</v>
+      </c>
+      <c r="H18">
+        <v>30.370443534379898</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>5000</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>7.70440253999999E-3</v>
+      </c>
+      <c r="G19">
+        <v>0.62593635018000005</v>
+      </c>
+      <c r="H19">
+        <v>62.062277821779901</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>5000</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>5.9140367799999996E-3</v>
+      </c>
+      <c r="G20">
+        <v>0.44917491786000002</v>
+      </c>
+      <c r="H20">
+        <v>31.666343097759999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>10000</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>2.4117075000000001E-3</v>
+      </c>
+      <c r="G21">
+        <v>4.9610627200000002E-3</v>
+      </c>
+      <c r="H21">
+        <v>0.18082493127999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>10000</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>1.8884328399999899E-3</v>
+      </c>
+      <c r="G22">
+        <v>9.8611054199999899E-3</v>
+      </c>
+      <c r="H22">
+        <v>0.75351090395999898</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>10000</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1.5417832E-3</v>
+      </c>
+      <c r="G23">
+        <v>1.3912809879999899E-2</v>
+      </c>
+      <c r="H23">
+        <v>0.24073645590000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>10000</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>4.6113191800000002E-3</v>
+      </c>
+      <c r="G24">
+        <v>0.47270693942000003</v>
+      </c>
+      <c r="H24">
+        <v>6.6725374729600002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>4.3559885999999897E-3</v>
+      </c>
+      <c r="G25">
+        <v>0.18076756699999999</v>
+      </c>
+      <c r="H25">
+        <v>23.604746588859999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>10000</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>10000</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>10000</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>10000</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>3.6966802E-4</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2.5333228000000001E-4</v>
+      </c>
+      <c r="H31" s="2">
+        <v>5.5116003999999895E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>500</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3.5961366000000002E-4</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2.2681951999999999E-4</v>
+      </c>
+      <c r="H32" s="2">
+        <v>7.0128569999999997E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>500</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3.5231887999999899E-4</v>
+      </c>
+      <c r="G33" s="2">
+        <v>2.5524498E-4</v>
+      </c>
+      <c r="H33" s="2">
+        <v>7.3267213999999995E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>500</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>7.0268319999999905E-4</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2.6027716399999899E-3</v>
+      </c>
+      <c r="H34">
+        <v>1.42274894599999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>500</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="F35" s="2">
+        <v>6.34715519999999E-4</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2.5250305199999998E-3</v>
+      </c>
+      <c r="H35">
+        <v>2.0724687459999998E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>500</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="F36" s="2">
+        <v>6.7341614000000001E-4</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2.8208762E-3</v>
+      </c>
+      <c r="H36">
+        <v>1.6236867320000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>500</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1.11711438E-3</v>
+      </c>
+      <c r="G37">
+        <v>1.184962904E-2</v>
+      </c>
+      <c r="H37">
+        <v>0.116301179239999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>500</v>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1.08528772E-3</v>
+      </c>
+      <c r="G38">
+        <v>1.1723907319999999E-2</v>
+      </c>
+      <c r="H38">
+        <v>0.12504765564</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>500</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.06420286E-3</v>
+      </c>
+      <c r="G39">
+        <v>1.1708410319999999E-2</v>
+      </c>
+      <c r="H39">
+        <v>0.122053745079999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>5000</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.4273371999999999E-3</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.5910181399999999E-3</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2.7587401399999899E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>5000</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1.3657035E-3</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.6336329E-3</v>
+      </c>
+      <c r="H41" s="2">
+        <v>4.4973114200000004E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>5000</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1.28853819999999E-3</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1.56385773999999E-3</v>
+      </c>
+      <c r="H42" s="2">
+        <v>4.6491934200000003E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>5000</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2">
+        <v>2.5861416400000002E-3</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1.22968358599999E-2</v>
+      </c>
+      <c r="H43">
+        <v>0.14510178539999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>5000</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2.6004418E-3</v>
+      </c>
+      <c r="G44">
+        <v>1.284344512E-2</v>
+      </c>
+      <c r="H44">
+        <v>0.14302093901999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>5000</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2.6502108999999999E-3</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1.3212455399999899E-2</v>
+      </c>
+      <c r="H45">
+        <v>0.172773514179999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>5000</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+      <c r="F46" s="2">
+        <v>4.02808518E-3</v>
+      </c>
+      <c r="G46">
+        <v>8.7610752580000006E-2</v>
+      </c>
+      <c r="H46">
+        <v>2.0340562132599902</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>5000</v>
+      </c>
+      <c r="D47">
+        <v>16</v>
+      </c>
+      <c r="F47">
+        <v>4.1581251399999998E-3</v>
+      </c>
+      <c r="G47">
+        <v>8.7963965300000002E-2</v>
+      </c>
+      <c r="H47">
+        <v>2.1219118204399998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>5000</v>
+      </c>
+      <c r="D48">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>5.29784137999999E-3</v>
+      </c>
+      <c r="G48">
+        <v>8.7727829679999897E-2</v>
+      </c>
+      <c r="H48">
+        <v>2.11668509493999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>10000</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1.8631521999999999E-3</v>
+      </c>
+      <c r="G49">
+        <v>1.8452106999999999E-3</v>
+      </c>
+      <c r="H49">
+        <v>5.6333308999999996E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>10000</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>2.0100169200000001E-3</v>
+      </c>
+      <c r="G50">
+        <v>1.9645734800000001E-3</v>
+      </c>
+      <c r="H50">
+        <v>5.9055875000000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>10000</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1.7373789399999901E-3</v>
+      </c>
+      <c r="G51">
+        <v>2.24958079999999E-3</v>
+      </c>
+      <c r="H51">
+        <v>5.2234269599999899E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>10000</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>3.48152468E-3</v>
+      </c>
+      <c r="G52">
+        <v>2.1977905799999999E-2</v>
+      </c>
+      <c r="H52">
+        <v>0.23102593653999901</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>10000</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>3.3286283400000001E-3</v>
+      </c>
+      <c r="G53">
+        <v>2.236076062E-2</v>
+      </c>
+      <c r="H53">
+        <v>0.26960134466000002</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>10000</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>10000</v>
+      </c>
+      <c r="D55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>10000</v>
+      </c>
+      <c r="D56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>10000</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D026784-D940-4903-8CB7-2720278E37DA}">
+  <dimension ref="B1:L57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.5876944000000002E-4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7.9256284000000002E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4.1356929600000003E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.1565359999999998E-4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0600658399999999E-3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3.2725067600000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.2936236000000001E-4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>8.2149167999999895E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7.4947991400000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.7298619800000001E-3</v>
+      </c>
+      <c r="G6">
+        <v>1.3592664359999901E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.35905098586</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.38233183999999E-3</v>
+      </c>
+      <c r="G7">
+        <v>1.3464357499999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.22416156273999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.6573229799999999E-3</v>
+      </c>
+      <c r="G8">
+        <v>1.0960183619999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.348906167759999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.9122570199999901E-3</v>
+      </c>
+      <c r="G9">
+        <v>7.6954921900000001E-2</v>
+      </c>
+      <c r="H9">
+        <v>4.5455594814999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.0190306999999996E-3</v>
+      </c>
+      <c r="G10">
+        <v>6.2438924399999998E-2</v>
+      </c>
+      <c r="H10">
+        <v>3.1230741166399998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>500</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3.7572284599999999E-3</v>
+      </c>
+      <c r="G11">
+        <v>0.10217573789999999</v>
+      </c>
+      <c r="H11">
+        <v>3.1659101450599998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>5000</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.8403088E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>9.9826660799999904E-3</v>
+      </c>
+      <c r="H12">
+        <v>0.19788447099999901</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>5000</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.1672005199999901E-3</v>
+      </c>
+      <c r="G13">
+        <v>1.23301889199999E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.15005009752000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5000</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.43711003999999E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4.0976655799999998E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.14273448331999899</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>5000</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.0968243600000002E-3</v>
+      </c>
+      <c r="G15">
+        <v>0.51169619704000002</v>
+      </c>
+      <c r="H15">
+        <v>21.77143943486</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>5000</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.180428964E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.486117203039999</v>
+      </c>
+      <c r="H16">
+        <v>17.604372304519998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>5000</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>8.6976958999999895E-3</v>
+      </c>
+      <c r="G17">
+        <v>0.239762657119999</v>
+      </c>
+      <c r="H17">
+        <v>12.861388567659899</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>5000</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>2.61877898E-2</v>
+      </c>
+      <c r="G18">
+        <v>1.05867466384</v>
+      </c>
+      <c r="H18">
+        <v>191.482833445599</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>5000</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>3.7883713440000001E-2</v>
+      </c>
+      <c r="G19">
+        <v>2.6210092739199999</v>
+      </c>
+      <c r="H19">
+        <v>170.114718766539</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>5000</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>3.110801346E-2</v>
+      </c>
+      <c r="G20">
+        <v>3.8391530351999998</v>
+      </c>
+      <c r="H20">
+        <v>147.98593053757901</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>10000</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>2.3514656999999999E-3</v>
+      </c>
+      <c r="G21">
+        <v>2.2404429399999998E-2</v>
+      </c>
+      <c r="H21">
+        <v>0.38844534936000003</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>10000</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>2.0911179399999901E-3</v>
+      </c>
+      <c r="G22">
+        <v>1.0020530779999899E-2</v>
+      </c>
+      <c r="H22">
+        <v>0.2332781498</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>10000</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1.89344384E-3</v>
+      </c>
+      <c r="G23">
+        <v>1.4931214700000001E-2</v>
+      </c>
+      <c r="H23">
+        <v>0.30746786787999902</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>10000</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>1.94913741E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.58877492872000003</v>
+      </c>
+      <c r="H24">
+        <v>40.923313784379999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>2.14361150599999E-2</v>
+      </c>
+      <c r="G25">
+        <v>0.98229310707999895</v>
+      </c>
+      <c r="H25">
+        <v>58.728886067859897</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>10000</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>10000</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>10000</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>10000</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>3.7222505999999999E-4</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4.7330465999999901E-4</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.3453178400000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>500</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3.6956543999999898E-4</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3.7257708000000003E-4</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.04205698E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>500</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3.8194827999999998E-4</v>
+      </c>
+      <c r="G33" s="2">
+        <v>4.2634809999999998E-4</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.3702455199999901E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>500</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.67962242E-3</v>
+      </c>
+      <c r="G34" s="2">
+        <v>8.4823998999999997E-3</v>
+      </c>
+      <c r="H34">
+        <v>5.8049505539999997E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>500</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.5254392999999901E-3</v>
+      </c>
+      <c r="G35" s="2">
+        <v>7.8104531399999996E-3</v>
+      </c>
+      <c r="H35">
+        <v>7.568579298E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>500</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1.64462208E-3</v>
+      </c>
+      <c r="G36" s="2">
+        <v>8.7058635999999901E-3</v>
+      </c>
+      <c r="H36">
+        <v>7.9085868500000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>500</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="F37" s="2">
+        <v>4.51761403999999E-3</v>
+      </c>
+      <c r="G37">
+        <v>6.2976501820000003E-2</v>
+      </c>
+      <c r="H37">
+        <v>1.1132623243599999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>500</v>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4.1471809599999904E-3</v>
+      </c>
+      <c r="G38">
+        <v>6.3980334379999906E-2</v>
+      </c>
+      <c r="H38">
+        <v>1.09470546585999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>500</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="F39" s="2">
+        <v>4.4299789399999999E-3</v>
+      </c>
+      <c r="G39">
+        <v>6.0236809999999898E-2</v>
+      </c>
+      <c r="H39">
+        <v>1.10148578874</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>5000</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.3202891999999999E-3</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2.1278682999999999E-3</v>
+      </c>
+      <c r="H40" s="2">
+        <v>7.4134531999999996E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>5000</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1.4090080799999999E-3</v>
+      </c>
+      <c r="G41" s="2">
+        <v>2.6585352000000001E-3</v>
+      </c>
+      <c r="H41" s="2">
+        <v>8.2336566799999997E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>5000</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1.3272004999999999E-3</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2.7353939199999998E-3</v>
+      </c>
+      <c r="H42" s="2">
+        <v>7.1501492199999902E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>5000</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2">
+        <v>9.4815279999999995E-3</v>
+      </c>
+      <c r="G43" s="2">
+        <v>7.4105083259999899E-2</v>
+      </c>
+      <c r="H43">
+        <v>0.75729544676000005</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>5000</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="F44" s="2">
+        <v>9.3923898599999993E-3</v>
+      </c>
+      <c r="G44">
+        <v>7.6336162839999999E-2</v>
+      </c>
+      <c r="H44">
+        <v>0.66982079175999998</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>5000</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2">
+        <v>8.9660317799999997E-3</v>
+      </c>
+      <c r="G45" s="2">
+        <v>7.0911824639999996E-2</v>
+      </c>
+      <c r="H45">
+        <v>0.689804475279999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>5000</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+      <c r="F46" s="2">
+        <v>3.6889225419999998E-2</v>
+      </c>
+      <c r="G46">
+        <v>0.62069029316000002</v>
+      </c>
+      <c r="H46">
+        <v>11.41930225728</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>5000</v>
+      </c>
+      <c r="D47">
+        <v>16</v>
+      </c>
+      <c r="F47">
+        <v>3.3966726879999999E-2</v>
+      </c>
+      <c r="G47">
+        <v>0.62639189334000001</v>
+      </c>
+      <c r="H47">
+        <v>10.8113482497599</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>5000</v>
+      </c>
+      <c r="D48">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>3.4026571419999999E-2</v>
+      </c>
+      <c r="G48">
+        <v>0.63841305191999997</v>
+      </c>
+      <c r="H48">
+        <v>11.70780505428</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>10000</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1.9577126799999998E-3</v>
+      </c>
+      <c r="G49">
+        <v>3.6716578599999901E-3</v>
+      </c>
+      <c r="H49">
+        <v>1.3292112599999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>10000</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>1.9712936800000001E-3</v>
+      </c>
+      <c r="G50">
+        <v>4.5979738799999999E-3</v>
+      </c>
+      <c r="H50">
+        <v>1.21706141399999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>10000</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1.8750758799999899E-3</v>
+      </c>
+      <c r="G51">
+        <v>3.7615601199999901E-3</v>
+      </c>
+      <c r="H51">
+        <v>1.149454862E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>10000</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>1.8039094499999998E-2</v>
+      </c>
+      <c r="G52">
+        <v>0.15665046839999899</v>
+      </c>
+      <c r="H52">
+        <v>1.5219997734199999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>10000</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>1.8166989079999901E-2</v>
+      </c>
+      <c r="G53">
+        <v>0.14204477124000001</v>
+      </c>
+      <c r="H53">
+        <v>1.3638920507800001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>10000</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>10000</v>
+      </c>
+      <c r="D55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>10000</v>
+      </c>
+      <c r="D56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>56</v>
       </c>

</xml_diff>